<commit_message>
AE-426 add missing translations to xlsx templates
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-2013-sv.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-2013-sv.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="1) etusivu" sheetId="1" state="visible" r:id="rId2"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="654">
   <si>
     <t xml:space="preserve">[:id]</t>
   </si>
@@ -1644,9 +1644,6 @@
     <t xml:space="preserve">med energiformsfaktor</t>
   </si>
   <si>
-    <t xml:space="preserve">kWh/vuosi</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -1676,7 +1673,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">/vuosi</t>
+      <t xml:space="preserve">/år</t>
     </r>
   </si>
   <si>
@@ -6672,13 +6669,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FFFF0000"/>
       </font>
@@ -6919,6 +6909,13 @@
       <font>
         <color rgb="FFFF0000"/>
       </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -9287,7 +9284,7 @@
   </sheetPr>
   <dimension ref="A1:AK262"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L49" activeCellId="0" sqref="L49"/>
     </sheetView>
   </sheetViews>
@@ -19096,7 +19093,7 @@
   </sheetPr>
   <dimension ref="A1:AC82"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="N15" activeCellId="0" sqref="N15"/>
     </sheetView>
   </sheetViews>
@@ -21935,8 +21932,8 @@
   </sheetPr>
   <dimension ref="A1:N94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A68" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F81" activeCellId="0" sqref="F81"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24333,8 +24330,8 @@
   </sheetPr>
   <dimension ref="A1:T113"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D80" activeCellId="0" sqref="D80"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24656,16 +24653,16 @@
       <c r="C16" s="249"/>
       <c r="D16" s="250"/>
       <c r="E16" s="251" t="s">
-        <v>337</v>
+        <v>106</v>
       </c>
       <c r="F16" s="251" t="s">
         <v>108</v>
       </c>
       <c r="G16" s="251" t="s">
+        <v>337</v>
+      </c>
+      <c r="H16" s="252" t="s">
         <v>338</v>
-      </c>
-      <c r="H16" s="252" t="s">
-        <v>339</v>
       </c>
       <c r="I16" s="181"/>
       <c r="J16" s="239"/>
@@ -24681,7 +24678,7 @@
     </row>
     <row r="17" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="159" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C17" s="173"/>
       <c r="D17" s="171"/>
@@ -24811,7 +24808,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="159" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C21" s="173"/>
       <c r="D21" s="253" t="s">
@@ -24957,7 +24954,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="159" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C25" s="173"/>
       <c r="D25" s="258" t="str">
@@ -24998,7 +24995,7 @@
       </c>
       <c r="C26" s="173"/>
       <c r="D26" s="259" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E26" s="260" t="str">
         <f aca="false">A42</f>
@@ -25053,7 +25050,7 @@
       </c>
       <c r="C28" s="167"/>
       <c r="D28" s="95" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E28" s="168"/>
       <c r="F28" s="168"/>
@@ -25096,7 +25093,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="159" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C30" s="173"/>
       <c r="D30" s="171"/>
@@ -25245,7 +25242,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="159" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C35" s="173"/>
       <c r="D35" s="262" t="str">
@@ -25333,7 +25330,7 @@
       </c>
       <c r="C38" s="167"/>
       <c r="D38" s="95" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E38" s="168"/>
       <c r="F38" s="168"/>
@@ -25375,19 +25372,19 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="159" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C40" s="173"/>
       <c r="D40" s="171"/>
       <c r="E40" s="171"/>
       <c r="F40" s="205" t="s">
+        <v>348</v>
+      </c>
+      <c r="G40" s="181" t="s">
         <v>349</v>
       </c>
-      <c r="G40" s="181" t="s">
+      <c r="H40" s="181" t="s">
         <v>350</v>
-      </c>
-      <c r="H40" s="181" t="s">
-        <v>351</v>
       </c>
       <c r="I40" s="181"/>
       <c r="J40" s="239"/>
@@ -25431,7 +25428,7 @@
     </row>
     <row r="42" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="159" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C42" s="173"/>
       <c r="D42" s="171"/>
@@ -25453,7 +25450,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="159" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C43" s="173"/>
       <c r="D43" s="174" t="s">
@@ -25477,11 +25474,11 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="159" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C44" s="173"/>
       <c r="D44" s="174" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E44" s="174"/>
       <c r="F44" s="254" t="str">
@@ -25509,11 +25506,11 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="159" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C45" s="173"/>
       <c r="D45" s="174" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E45" s="174"/>
       <c r="F45" s="188" t="str">
@@ -25541,11 +25538,11 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="159" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C46" s="173"/>
       <c r="D46" s="174" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E46" s="174"/>
       <c r="F46" s="188" t="str">
@@ -25573,11 +25570,11 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="159" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C47" s="173"/>
       <c r="D47" s="174" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E47" s="174"/>
       <c r="F47" s="188" t="str">
@@ -25604,7 +25601,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="159" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C48" s="173"/>
       <c r="D48" s="174" t="s">
@@ -25637,11 +25634,11 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="159" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C49" s="173"/>
       <c r="D49" s="174" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E49" s="174"/>
       <c r="F49" s="188" t="str">
@@ -25668,11 +25665,11 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="159" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C50" s="173"/>
       <c r="D50" s="259" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E50" s="259"/>
       <c r="F50" s="267" t="str">
@@ -25701,11 +25698,11 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="159" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C51" s="173"/>
       <c r="D51" s="268" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E51" s="259"/>
       <c r="F51" s="225"/>
@@ -25725,7 +25722,7 @@
     </row>
     <row r="52" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="159" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C52" s="173"/>
       <c r="D52" s="178"/>
@@ -25747,11 +25744,11 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="159" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C53" s="167"/>
       <c r="D53" s="95" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E53" s="168"/>
       <c r="F53" s="168"/>
@@ -25762,7 +25759,7 @@
     </row>
     <row r="54" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="159" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C54" s="173"/>
       <c r="D54" s="178"/>
@@ -25775,7 +25772,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="159" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C55" s="173"/>
       <c r="D55" s="171"/>
@@ -25791,7 +25788,7 @@
     </row>
     <row r="56" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="159" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C56" s="173"/>
       <c r="D56" s="171"/>
@@ -25803,11 +25800,11 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="159" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C57" s="173"/>
       <c r="D57" s="174" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E57" s="174"/>
       <c r="F57" s="223" t="str">
@@ -25824,11 +25821,11 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="159" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C58" s="173"/>
       <c r="D58" s="174" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E58" s="174"/>
       <c r="F58" s="223" t="str">
@@ -25845,7 +25842,7 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="159" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C59" s="173"/>
       <c r="D59" s="174" t="s">
@@ -25866,11 +25863,11 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="159" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C60" s="173"/>
       <c r="D60" s="174" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E60" s="174"/>
       <c r="F60" s="223" t="str">
@@ -25887,7 +25884,7 @@
     </row>
     <row r="61" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="159" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C61" s="173"/>
       <c r="D61" s="174"/>
@@ -25900,11 +25897,11 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="159" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C62" s="173"/>
       <c r="D62" s="222" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E62" s="222"/>
       <c r="F62" s="222"/>
@@ -25915,11 +25912,11 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="159" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C63" s="173"/>
       <c r="D63" s="222" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E63" s="222"/>
       <c r="F63" s="222"/>
@@ -25930,7 +25927,7 @@
     </row>
     <row r="64" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="159" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C64" s="173"/>
       <c r="D64" s="174"/>
@@ -25943,11 +25940,11 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="159" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C65" s="167"/>
       <c r="D65" s="95" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E65" s="168"/>
       <c r="F65" s="168"/>
@@ -25958,7 +25955,7 @@
     </row>
     <row r="66" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="159" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C66" s="173"/>
       <c r="D66" s="178"/>
@@ -25971,7 +25968,7 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="159" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C67" s="173"/>
       <c r="D67" s="171"/>
@@ -25987,7 +25984,7 @@
     </row>
     <row r="68" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="159" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C68" s="173"/>
       <c r="D68" s="171"/>
@@ -25999,11 +25996,11 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="159" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C69" s="173"/>
       <c r="D69" s="196" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E69" s="196"/>
       <c r="F69" s="223" t="str">
@@ -26020,7 +26017,7 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="159" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C70" s="173"/>
       <c r="D70" s="196" t="s">
@@ -26041,11 +26038,11 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="159" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C71" s="173"/>
       <c r="D71" s="174" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E71" s="174"/>
       <c r="F71" s="223" t="str">
@@ -26062,7 +26059,7 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="159" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C72" s="173"/>
       <c r="D72" s="174" t="s">
@@ -26083,11 +26080,11 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="159" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C73" s="173"/>
       <c r="D73" s="174" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E73" s="174"/>
       <c r="F73" s="223" t="str">
@@ -26104,7 +26101,7 @@
     </row>
     <row r="74" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="159" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C74" s="173"/>
       <c r="D74" s="174"/>
@@ -26117,11 +26114,11 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="159" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C75" s="167"/>
       <c r="D75" s="95" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E75" s="168"/>
       <c r="F75" s="168"/>
@@ -26132,7 +26129,7 @@
     </row>
     <row r="76" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="159" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C76" s="173"/>
       <c r="D76" s="178"/>
@@ -26145,11 +26142,11 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="159" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C77" s="173"/>
       <c r="D77" s="174" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E77" s="174"/>
       <c r="F77" s="269" t="str">
@@ -26163,7 +26160,7 @@
     </row>
     <row r="78" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="159" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C78" s="229"/>
       <c r="D78" s="230"/>
@@ -26176,177 +26173,177 @@
     </row>
     <row r="79" customFormat="false" ht="5.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="159" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="159" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="159" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="159" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="159" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="159" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="159" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="159" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="159" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="159" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="159" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="159" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="159" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="159" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="159" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="159" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="159" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="159" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="159" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="159" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="159" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="159" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="159" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="159" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="159" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="159" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="159" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="159" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="159" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="159" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="159" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="159" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="159" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="159" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="159" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
   </sheetData>
@@ -26406,87 +26403,87 @@
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E16">
+  <conditionalFormatting sqref="F40:H40 F42:H42">
     <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="214">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F40:H40 F42:H42">
+  <conditionalFormatting sqref="F50:H51">
     <cfRule type="cellIs" priority="7" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="215">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F50:H51">
+  <conditionalFormatting sqref="H50:H51">
     <cfRule type="cellIs" priority="8" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="216">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F50:F51 F50:H50">
+    <cfRule type="cellIs" priority="9" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="217">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G50:G51">
+    <cfRule type="cellIs" priority="10" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="218">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D64">
+    <cfRule type="cellIs" priority="11" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="219">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F31:G31 F30">
+    <cfRule type="cellIs" priority="12" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="220">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H63">
+    <cfRule type="cellIs" priority="13" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="221">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F9:F10">
+    <cfRule type="cellIs" priority="14" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="222">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10">
+    <cfRule type="cellIs" priority="15" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="223">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D25">
+    <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="224">
+      <formula>LEFT(D25,1)="*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D26">
+    <cfRule type="cellIs" priority="17" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="225">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G30 F41:H41 G55 G67">
+    <cfRule type="cellIs" priority="18" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="226">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D50:D51">
+    <cfRule type="cellIs" priority="19" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="227">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D43:D49">
+    <cfRule type="cellIs" priority="20" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="228">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G50:G51">
+    <cfRule type="cellIs" priority="21" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="229">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="H50:H51">
-    <cfRule type="cellIs" priority="9" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="217">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F50:F51 F50:H50">
-    <cfRule type="cellIs" priority="10" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="218">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G50:G51">
-    <cfRule type="cellIs" priority="11" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="219">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D64">
-    <cfRule type="cellIs" priority="12" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="220">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F31:G31 F30">
-    <cfRule type="cellIs" priority="13" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="221">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H63">
-    <cfRule type="cellIs" priority="14" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="222">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F9:F10">
-    <cfRule type="cellIs" priority="15" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="223">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" priority="16" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="224">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D25">
-    <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="225">
-      <formula>LEFT(D25,1)="*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D26">
-    <cfRule type="cellIs" priority="18" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="226">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G30 F41:H41 G55 G67">
-    <cfRule type="cellIs" priority="19" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="227">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D50:D51">
-    <cfRule type="cellIs" priority="20" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="228">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D43:D49">
-    <cfRule type="cellIs" priority="21" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="229">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G50:G51">
     <cfRule type="cellIs" priority="22" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="230">
       <formula>"*"</formula>
     </cfRule>
@@ -26496,77 +26493,77 @@
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H50:H51">
+  <conditionalFormatting sqref="G43">
     <cfRule type="cellIs" priority="24" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="232">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G43">
+  <conditionalFormatting sqref="H43">
     <cfRule type="cellIs" priority="25" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="233">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H43">
+  <conditionalFormatting sqref="H61:H62">
     <cfRule type="cellIs" priority="26" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="234">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H61:H62">
+      <formula>"Täytä lähtötietoihin!"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F56 G61">
     <cfRule type="cellIs" priority="27" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="235">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F61">
+    <cfRule type="cellIs" priority="28" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="236">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G56 F55">
+    <cfRule type="cellIs" priority="29" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="237">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F61">
+    <cfRule type="cellIs" priority="30" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="238">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G68">
+    <cfRule type="cellIs" priority="31" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="239">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D57:D61">
+    <cfRule type="cellIs" priority="32" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="240">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D62:D63">
+    <cfRule type="cellIs" priority="33" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="241">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65:H66 E74:H74">
+    <cfRule type="cellIs" priority="34" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="242">
       <formula>"Täytä lähtötietoihin!"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F56 G61">
-    <cfRule type="cellIs" priority="28" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="236">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F61">
-    <cfRule type="cellIs" priority="29" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="237">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G56 F55">
-    <cfRule type="cellIs" priority="30" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="238">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F61">
-    <cfRule type="cellIs" priority="31" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="239">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G68">
-    <cfRule type="cellIs" priority="32" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="240">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D57:D61">
-    <cfRule type="cellIs" priority="33" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="241">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D62:D63">
-    <cfRule type="cellIs" priority="34" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="242">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C65:H66 E74:H74">
+  <conditionalFormatting sqref="D74">
     <cfRule type="cellIs" priority="35" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="243">
-      <formula>"Täytä lähtötietoihin!"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D74">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F68">
     <cfRule type="cellIs" priority="36" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="244">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F68">
+  <conditionalFormatting sqref="D70:D71 D73">
     <cfRule type="cellIs" priority="37" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="245">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D70:D71 D73">
+  <conditionalFormatting sqref="F77">
     <cfRule type="cellIs" priority="38" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="246">
       <formula>"*"</formula>
     </cfRule>
@@ -26576,57 +26573,57 @@
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F77">
+  <conditionalFormatting sqref="D77">
     <cfRule type="cellIs" priority="40" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="248">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D77">
+  <conditionalFormatting sqref="F17">
     <cfRule type="cellIs" priority="41" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="249">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F17">
+  <conditionalFormatting sqref="E17">
     <cfRule type="cellIs" priority="42" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="250">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E17">
+  <conditionalFormatting sqref="E26">
     <cfRule type="cellIs" priority="43" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="251">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E26">
+  <conditionalFormatting sqref="F26">
     <cfRule type="cellIs" priority="44" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="252">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F26">
+  <conditionalFormatting sqref="J3 J8 J11 J13 J15 J17 J19 J21 J25 J27 J29 J31 J33 J35 J37 J39 J41 J43 J45 J47 J49 J51 J53 J55 J57 J59 J61 J63 J65 J67 J69 J71:J72 J74 J76 J78">
     <cfRule type="cellIs" priority="45" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="253">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3 J8 J11 J13 J15 J17 J19 J21 J25 J27 J29 J31 J33 J35 J37 J39 J41 J43 J45 J47 J49 J51 J53 J55 J57 J59 J61 J63 J65 J67 J69 J71:J72 J74 J76 J78">
+  <conditionalFormatting sqref="J4:J7 J9:J10 J12 J14 J16 J18 J20 J22:J24 J26 J28 J30 J32 J34 J36 J38 J40 J42 J44 J46 J48 J50 J52 J54 J56 J58 J60 J62 J64 J66 J68 J70 J73 J75 J77">
     <cfRule type="cellIs" priority="46" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="254">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J4:J7 J9:J10 J12 J14 J16 J18 J20 J22:J24 J26 J28 J30 J32 J34 J36 J38 J40 J42 J44 J46 J48 J50 J52 J54 J56 J58 J60 J62 J64 J66 J68 J70 J73 J75 J77">
+  <conditionalFormatting sqref="I12:I14 I16:I18 I20:I24 I26:I28 I30:I32 I34:I36 I38:I40 I42:I44 I46:I48 I50:I52 I54:I56 I58:I60 I62:I64 I66:I68 I70:I73 I75:I77">
     <cfRule type="cellIs" priority="47" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="255">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I12:I14 I16:I18 I20:I24 I26:I28 I30:I32 I34:I36 I38:I40 I42:I44 I46:I48 I50:I52 I54:I56 I58:I60 I62:I64 I66:I68 I70:I73 I75:I77">
+  <conditionalFormatting sqref="I3 I8 I11 I15 I19 I25 I29 I33 I37 I41 I45 I49 I53 I57 I61 I65 I69 I74 I78">
     <cfRule type="cellIs" priority="48" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="256">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3 I8 I11 I15 I19 I25 I29 I33 I37 I41 I45 I49 I53 I57 I61 I65 I69 I74 I78">
+  <conditionalFormatting sqref="I2">
     <cfRule type="cellIs" priority="49" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="257">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
+  <conditionalFormatting sqref="H32:H36">
     <cfRule type="cellIs" priority="50" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="258">
       <formula>"*"</formula>
     </cfRule>
@@ -26636,57 +26633,57 @@
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H32:H36">
+  <conditionalFormatting sqref="H67:H68">
     <cfRule type="cellIs" priority="52" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="260">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H67:H68">
+  <conditionalFormatting sqref="H69:H73">
     <cfRule type="cellIs" priority="53" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="261">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H69:H73">
+  <conditionalFormatting sqref="H56 H58 H60">
     <cfRule type="cellIs" priority="54" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="262">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H56 H58 H60">
+  <conditionalFormatting sqref="H55 H57 H59">
     <cfRule type="cellIs" priority="55" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="263">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H55 H57 H59">
+  <conditionalFormatting sqref="F18:F25 H20">
     <cfRule type="cellIs" priority="56" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="264">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F18:F25 H20">
+  <conditionalFormatting sqref="G32:G36">
     <cfRule type="cellIs" priority="57" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="265">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G32:G36">
+  <conditionalFormatting sqref="E8">
     <cfRule type="cellIs" priority="58" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="266">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E8">
+  <conditionalFormatting sqref="E5 E8">
     <cfRule type="cellIs" priority="59" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="267">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E5 E8">
+      <formula>"Täytä etusivulle!"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D72">
     <cfRule type="cellIs" priority="60" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="268">
-      <formula>"Täytä etusivulle!"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D72">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G26">
     <cfRule type="cellIs" priority="61" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="269">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G26">
+  <conditionalFormatting sqref="H26">
     <cfRule type="cellIs" priority="62" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="270">
       <formula>"*"</formula>
     </cfRule>
@@ -26696,176 +26693,176 @@
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H26">
+  <conditionalFormatting sqref="G21:G25 G18:G19">
     <cfRule type="cellIs" priority="64" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="272">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G21:G25 G18:G19">
+  <conditionalFormatting sqref="H21:H25 H18:H19">
     <cfRule type="cellIs" priority="65" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="273">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H21:H25 H18:H19">
+  <conditionalFormatting sqref="G50:H50">
     <cfRule type="cellIs" priority="66" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="274">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G50:H50">
+  <conditionalFormatting sqref="G57:G60">
     <cfRule type="cellIs" priority="67" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="275">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G57:G60">
+  <conditionalFormatting sqref="G69:G73">
     <cfRule type="cellIs" priority="68" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="276">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G69:G73">
+  <conditionalFormatting sqref="E18">
     <cfRule type="cellIs" priority="69" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="277">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E18">
+  <conditionalFormatting sqref="E19:E25 G20">
     <cfRule type="cellIs" priority="70" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="278">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E19:E25 G20">
+  <conditionalFormatting sqref="D9">
     <cfRule type="cellIs" priority="71" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="279">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D9">
+  <conditionalFormatting sqref="N22:O24">
     <cfRule type="cellIs" priority="72" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="280">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N22:O24">
+  <conditionalFormatting sqref="F67">
     <cfRule type="cellIs" priority="73" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="281">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F67">
+  <conditionalFormatting sqref="F69">
     <cfRule type="cellIs" priority="74" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="282">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F69">
+  <conditionalFormatting sqref="F70:F73">
     <cfRule type="cellIs" priority="75" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="283">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F70:F73">
+  <conditionalFormatting sqref="F57">
     <cfRule type="cellIs" priority="76" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="284">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F57">
+  <conditionalFormatting sqref="F58:F60">
     <cfRule type="cellIs" priority="77" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="285">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F58:F60">
+  <conditionalFormatting sqref="F45:F49">
     <cfRule type="cellIs" priority="78" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="286">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F45:F49">
+  <conditionalFormatting sqref="G44:G46">
     <cfRule type="cellIs" priority="79" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="287">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G44:G46">
+  <conditionalFormatting sqref="G48">
     <cfRule type="cellIs" priority="80" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="288">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G48">
+  <conditionalFormatting sqref="H48">
     <cfRule type="cellIs" priority="81" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="289">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H48">
+  <conditionalFormatting sqref="F36">
     <cfRule type="cellIs" priority="82" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="290">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F36">
+  <conditionalFormatting sqref="F35">
     <cfRule type="cellIs" priority="83" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="291">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F35">
+  <conditionalFormatting sqref="F34">
     <cfRule type="cellIs" priority="84" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="292">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F34">
+  <conditionalFormatting sqref="F33">
     <cfRule type="cellIs" priority="85" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="293">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F33">
+  <conditionalFormatting sqref="F32">
     <cfRule type="cellIs" priority="86" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="294">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F32">
-    <cfRule type="cellIs" priority="87" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="295">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="D22:D24">
-    <cfRule type="expression" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="148">
+    <cfRule type="expression" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="148">
       <formula>LEFT(D22,1)="*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20:D21">
-    <cfRule type="expression" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="182">
+    <cfRule type="expression" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="182">
       <formula>LEFT(D20,1)="*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F44">
-    <cfRule type="cellIs" priority="90" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="296">
+    <cfRule type="cellIs" priority="89" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="295">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H44">
-    <cfRule type="cellIs" priority="91" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="159">
+    <cfRule type="cellIs" priority="90" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="159">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G47:H47 G49:H49">
-    <cfRule type="cellIs" priority="92" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="160">
+    <cfRule type="cellIs" priority="91" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="160">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H45:H46">
-    <cfRule type="cellIs" priority="93" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="164">
+    <cfRule type="cellIs" priority="92" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="164">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31:D36">
-    <cfRule type="cellIs" priority="94" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="185">
+    <cfRule type="cellIs" priority="93" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="185">
       <formula>"tyhjä"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="95" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="186">
+    <cfRule type="cellIs" priority="94" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="186">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31:D36">
-    <cfRule type="cellIs" priority="96" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="187">
+    <cfRule type="cellIs" priority="95" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="187">
       <formula>"- Valitse -"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18:D19">
-    <cfRule type="expression" priority="97" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="185">
+    <cfRule type="expression" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="185">
       <formula>LEFT(D18,1)="*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D69:D70">
-    <cfRule type="cellIs" priority="98" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="181">
+    <cfRule type="cellIs" priority="97" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="181">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E16">
+    <cfRule type="cellIs" priority="98" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="296">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26916,11 +26913,11 @@
     </row>
     <row r="2" s="271" customFormat="true" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="270" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C2" s="272"/>
       <c r="D2" s="273" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E2" s="273"/>
       <c r="F2" s="274"/>
@@ -26932,11 +26929,11 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="91" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C3" s="98"/>
       <c r="D3" s="24" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E3" s="276"/>
       <c r="F3" s="14"/>
@@ -26948,7 +26945,7 @@
     </row>
     <row r="4" customFormat="false" ht="7.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="91" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C4" s="98"/>
       <c r="D4" s="14"/>
@@ -26962,11 +26959,11 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="91" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C5" s="94"/>
       <c r="D5" s="95" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E5" s="95"/>
       <c r="F5" s="96"/>
@@ -26978,7 +26975,7 @@
     </row>
     <row r="6" customFormat="false" ht="3.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="91" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C6" s="98"/>
       <c r="D6" s="14"/>
@@ -26992,7 +26989,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="91" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C7" s="98"/>
       <c r="D7" s="62" t="str">
@@ -27007,7 +27004,7 @@
     </row>
     <row r="8" customFormat="false" ht="3.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="91" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C8" s="98"/>
       <c r="D8" s="14"/>
@@ -27020,7 +27017,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="91" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C9" s="98"/>
       <c r="D9" s="14"/>
@@ -27034,11 +27031,11 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="91" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C10" s="98"/>
       <c r="D10" s="62" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="278"/>
@@ -27054,7 +27051,7 @@
     </row>
     <row r="11" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="91" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C11" s="98"/>
       <c r="D11" s="14"/>
@@ -27068,11 +27065,11 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="91" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C12" s="98"/>
       <c r="D12" s="287" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E12" s="287"/>
       <c r="F12" s="288"/>
@@ -27091,11 +27088,11 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="91" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C13" s="98"/>
       <c r="D13" s="287" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="E13" s="287"/>
       <c r="F13" s="288"/>
@@ -27114,11 +27111,11 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="91" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C14" s="98"/>
       <c r="D14" s="279" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E14" s="287"/>
       <c r="F14" s="288"/>
@@ -27137,11 +27134,11 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="91" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C15" s="98"/>
       <c r="D15" s="279" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E15" s="287"/>
       <c r="F15" s="288"/>
@@ -27160,11 +27157,11 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="91" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C16" s="98"/>
       <c r="D16" s="287" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E16" s="287"/>
       <c r="F16" s="287"/>
@@ -27183,7 +27180,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="91" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C17" s="98"/>
       <c r="D17" s="294" t="str">
@@ -27207,7 +27204,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="91" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C18" s="98"/>
       <c r="D18" s="294" t="str">
@@ -27231,7 +27228,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="91" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C19" s="98"/>
       <c r="D19" s="294" t="str">
@@ -27255,7 +27252,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="91" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C20" s="98"/>
       <c r="D20" s="294" t="str">
@@ -27279,7 +27276,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="91" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C21" s="98"/>
       <c r="D21" s="294" t="str">
@@ -27303,7 +27300,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="91" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C22" s="98"/>
       <c r="D22" s="295"/>
@@ -27321,7 +27318,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="91" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C23" s="98"/>
       <c r="D23" s="299"/>
@@ -27336,21 +27333,21 @@
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="91" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C24" s="98"/>
       <c r="D24" s="302" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E24" s="302"/>
       <c r="F24" s="303" t="s">
+        <v>472</v>
+      </c>
+      <c r="G24" s="304" t="s">
         <v>473</v>
       </c>
-      <c r="G24" s="304" t="s">
+      <c r="H24" s="303" t="s">
         <v>474</v>
-      </c>
-      <c r="H24" s="303" t="s">
-        <v>475</v>
       </c>
       <c r="I24" s="304" t="s">
         <v>106</v>
@@ -27363,7 +27360,7 @@
     </row>
     <row r="25" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="91" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C25" s="98"/>
       <c r="D25" s="62"/>
@@ -27378,11 +27375,11 @@
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="91" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C26" s="98"/>
       <c r="D26" s="287" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="E26" s="287"/>
       <c r="F26" s="291" t="str">
@@ -27390,7 +27387,7 @@
         <v>[:toteutunut-ostoenergiankulutus :ostetut-polttoaineet :kevyt-polttooljy]</v>
       </c>
       <c r="G26" s="308" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="H26" s="281" t="n">
         <v>10</v>
@@ -27408,11 +27405,11 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="91" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C27" s="98"/>
       <c r="D27" s="287" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E27" s="287"/>
       <c r="F27" s="291" t="str">
@@ -27420,7 +27417,7 @@
         <v>[:toteutunut-ostoenergiankulutus :ostetut-polttoaineet :pilkkeet-havu-sekapuu]</v>
       </c>
       <c r="G27" s="308" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="H27" s="281" t="n">
         <v>1300</v>
@@ -27438,11 +27435,11 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="91" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C28" s="98"/>
       <c r="D28" s="287" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E28" s="287"/>
       <c r="F28" s="291" t="str">
@@ -27450,7 +27447,7 @@
         <v>[:toteutunut-ostoenergiankulutus :ostetut-polttoaineet :pilkkeet-koivu]</v>
       </c>
       <c r="G28" s="308" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="H28" s="281" t="n">
         <v>1700</v>
@@ -27468,11 +27465,11 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="91" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C29" s="98"/>
       <c r="D29" s="287" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E29" s="287"/>
       <c r="F29" s="291" t="str">
@@ -27480,7 +27477,7 @@
         <v>[:toteutunut-ostoenergiankulutus :ostetut-polttoaineet :puupelletit]</v>
       </c>
       <c r="G29" s="308" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="H29" s="281" t="n">
         <v>4.7</v>
@@ -27498,7 +27495,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="91" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C30" s="98"/>
       <c r="D30" s="312" t="str">
@@ -27531,7 +27528,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="91" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C31" s="98"/>
       <c r="D31" s="312" t="str">
@@ -27564,7 +27561,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="91" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C32" s="98"/>
       <c r="D32" s="315"/>
@@ -27585,7 +27582,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="91" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C33" s="98"/>
       <c r="D33" s="315"/>
@@ -27606,7 +27603,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="91" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C34" s="98"/>
       <c r="D34" s="315"/>
@@ -27627,7 +27624,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="91" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C35" s="98"/>
       <c r="D35" s="315"/>
@@ -27648,7 +27645,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="91" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C36" s="98"/>
       <c r="D36" s="315"/>
@@ -27669,7 +27666,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="91" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C37" s="98"/>
       <c r="D37" s="315"/>
@@ -27690,7 +27687,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="91" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C38" s="98"/>
       <c r="D38" s="315"/>
@@ -27711,7 +27708,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="91" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C39" s="98"/>
       <c r="D39" s="315"/>
@@ -27732,7 +27729,7 @@
     </row>
     <row r="40" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="91" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C40" s="98"/>
       <c r="D40" s="299"/>
@@ -27747,11 +27744,11 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="91" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C41" s="98"/>
       <c r="D41" s="317" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E41" s="299"/>
       <c r="F41" s="288"/>
@@ -27764,7 +27761,7 @@
     </row>
     <row r="42" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="91" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C42" s="98"/>
       <c r="D42" s="318"/>
@@ -27779,7 +27776,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="91" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C43" s="98"/>
       <c r="D43" s="299"/>
@@ -27794,11 +27791,11 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="91" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C44" s="98"/>
       <c r="D44" s="62" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="E44" s="299"/>
       <c r="F44" s="288"/>
@@ -27811,7 +27808,7 @@
     </row>
     <row r="45" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="91" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C45" s="98"/>
       <c r="D45" s="62"/>
@@ -27826,7 +27823,7 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="91" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C46" s="98"/>
       <c r="D46" s="62"/>
@@ -27845,11 +27842,11 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="91" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C47" s="98"/>
       <c r="D47" s="24" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E47" s="24"/>
       <c r="F47" s="323"/>
@@ -27868,11 +27865,11 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="91" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C48" s="98"/>
       <c r="D48" s="24" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E48" s="24"/>
       <c r="F48" s="323"/>
@@ -27891,11 +27888,11 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="91" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C49" s="98"/>
       <c r="D49" s="24" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E49" s="24"/>
       <c r="F49" s="323"/>
@@ -27914,11 +27911,11 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="91" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C50" s="98"/>
       <c r="D50" s="24" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E50" s="24"/>
       <c r="F50" s="323"/>
@@ -27937,11 +27934,11 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="91" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C51" s="98"/>
       <c r="D51" s="62" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E51" s="62"/>
       <c r="F51" s="14"/>
@@ -27959,7 +27956,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="91" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C52" s="98"/>
       <c r="D52" s="62"/>
@@ -27973,11 +27970,11 @@
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="91" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C53" s="98"/>
       <c r="D53" s="143" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E53" s="143"/>
       <c r="F53" s="143"/>
@@ -27989,7 +27986,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="91" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C54" s="98"/>
       <c r="D54" s="143"/>
@@ -28003,7 +28000,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="91" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C55" s="98"/>
       <c r="D55" s="143"/>
@@ -28017,7 +28014,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="91" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C56" s="98"/>
       <c r="D56" s="143"/>
@@ -28031,7 +28028,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="91" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C57" s="98"/>
       <c r="D57" s="143"/>
@@ -28045,7 +28042,7 @@
     </row>
     <row r="58" customFormat="false" ht="3.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="91" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C58" s="144"/>
       <c r="D58" s="145"/>
@@ -28060,47 +28057,47 @@
     </row>
     <row r="59" customFormat="false" ht="4.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="91" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="91" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="91" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="91" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="91" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="91" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="91" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="91" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="91" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
   </sheetData>
@@ -28817,10 +28814,10 @@
     </row>
     <row r="2" s="329" customFormat="true" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="328" t="s">
+        <v>531</v>
+      </c>
+      <c r="C2" s="330" t="s">
         <v>532</v>
-      </c>
-      <c r="C2" s="330" t="s">
-        <v>533</v>
       </c>
       <c r="D2" s="330"/>
       <c r="E2" s="330"/>
@@ -28829,7 +28826,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="151" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C3" s="331" t="s">
         <v>152</v>
@@ -28841,7 +28838,7 @@
     </row>
     <row r="4" customFormat="false" ht="7.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="327" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C4" s="144"/>
       <c r="D4" s="5"/>
@@ -28851,13 +28848,13 @@
     </row>
     <row r="5" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="327" t="s">
+        <v>535</v>
+      </c>
+      <c r="C5" s="332" t="s">
         <v>536</v>
       </c>
-      <c r="C5" s="332" t="s">
+      <c r="D5" s="95" t="s">
         <v>537</v>
-      </c>
-      <c r="D5" s="95" t="s">
-        <v>538</v>
       </c>
       <c r="E5" s="168"/>
       <c r="F5" s="168"/>
@@ -28865,7 +28862,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="327" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C6" s="333" t="str">
         <f aca="false">A3</f>
@@ -28878,7 +28875,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="327" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C7" s="333"/>
       <c r="D7" s="333"/>
@@ -28888,7 +28885,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="327" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C8" s="333"/>
       <c r="D8" s="333"/>
@@ -28898,7 +28895,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="327" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C9" s="333"/>
       <c r="D9" s="333"/>
@@ -28908,7 +28905,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="327" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C10" s="333"/>
       <c r="D10" s="333"/>
@@ -28918,7 +28915,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="327" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C11" s="333"/>
       <c r="D11" s="333"/>
@@ -28928,7 +28925,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="327" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C12" s="333"/>
       <c r="D12" s="333"/>
@@ -28938,7 +28935,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="327" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C13" s="333"/>
       <c r="D13" s="333"/>
@@ -28948,7 +28945,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="327" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C14" s="333"/>
       <c r="D14" s="333"/>
@@ -28958,7 +28955,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="327" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C15" s="333"/>
       <c r="D15" s="333"/>
@@ -28968,10 +28965,10 @@
     </row>
     <row r="16" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="151" t="s">
+        <v>548</v>
+      </c>
+      <c r="C16" s="334" t="s">
         <v>549</v>
-      </c>
-      <c r="C16" s="334" t="s">
-        <v>550</v>
       </c>
       <c r="D16" s="334"/>
       <c r="E16" s="334"/>
@@ -28980,7 +28977,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="151" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C17" s="335" t="n">
         <v>1</v>
@@ -28995,7 +28992,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="151" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C18" s="335" t="n">
         <v>2</v>
@@ -29010,7 +29007,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="151" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C19" s="335" t="n">
         <v>3</v>
@@ -29025,25 +29022,25 @@
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="151" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C20" s="337"/>
       <c r="D20" s="338" t="s">
+        <v>554</v>
+      </c>
+      <c r="E20" s="338" t="s">
         <v>555</v>
       </c>
-      <c r="E20" s="338" t="s">
+      <c r="F20" s="338" t="s">
         <v>556</v>
       </c>
-      <c r="F20" s="338" t="s">
+      <c r="G20" s="339" t="s">
         <v>557</v>
-      </c>
-      <c r="G20" s="339" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="151" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C21" s="337"/>
       <c r="D21" s="109" t="s">
@@ -29056,12 +29053,12 @@
         <v>106</v>
       </c>
       <c r="G21" s="109" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="151" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C22" s="335" t="n">
         <v>1</v>
@@ -29085,7 +29082,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="151" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C23" s="335" t="n">
         <v>2</v>
@@ -29109,7 +29106,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="151" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C24" s="335" t="n">
         <v>3</v>
@@ -29133,10 +29130,10 @@
     </row>
     <row r="25" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="151" t="s">
+        <v>563</v>
+      </c>
+      <c r="C25" s="341" t="s">
         <v>564</v>
-      </c>
-      <c r="C25" s="341" t="s">
-        <v>565</v>
       </c>
       <c r="D25" s="95"/>
       <c r="E25" s="168"/>
@@ -29145,7 +29142,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="151" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C26" s="333" t="str">
         <f aca="false">A23</f>
@@ -29158,7 +29155,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="151" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C27" s="333"/>
       <c r="D27" s="333"/>
@@ -29168,7 +29165,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="151" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C28" s="333"/>
       <c r="D28" s="333"/>
@@ -29178,7 +29175,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="151" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C29" s="333"/>
       <c r="D29" s="333"/>
@@ -29188,7 +29185,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="151" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C30" s="333"/>
       <c r="D30" s="333"/>
@@ -29198,7 +29195,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="151" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C31" s="333"/>
       <c r="D31" s="333"/>
@@ -29208,7 +29205,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="151" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C32" s="333"/>
       <c r="D32" s="333"/>
@@ -29218,7 +29215,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="151" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C33" s="333"/>
       <c r="D33" s="333"/>
@@ -29228,7 +29225,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="151" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C34" s="333"/>
       <c r="D34" s="333"/>
@@ -29238,7 +29235,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="151" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C35" s="333"/>
       <c r="D35" s="333"/>
@@ -29248,10 +29245,10 @@
     </row>
     <row r="36" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="151" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C36" s="334" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D36" s="334"/>
       <c r="E36" s="334"/>
@@ -29260,7 +29257,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="151" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C37" s="335" t="n">
         <v>1</v>
@@ -29275,7 +29272,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="151" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C38" s="335" t="n">
         <v>2</v>
@@ -29290,7 +29287,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="151" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C39" s="335" t="n">
         <v>3</v>
@@ -29305,25 +29302,25 @@
     </row>
     <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="151" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C40" s="337"/>
       <c r="D40" s="338" t="s">
+        <v>554</v>
+      </c>
+      <c r="E40" s="338" t="s">
         <v>555</v>
       </c>
-      <c r="E40" s="338" t="s">
+      <c r="F40" s="338" t="s">
         <v>556</v>
       </c>
-      <c r="F40" s="338" t="s">
+      <c r="G40" s="339" t="s">
         <v>557</v>
-      </c>
-      <c r="G40" s="339" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="151" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C41" s="337"/>
       <c r="D41" s="109" t="s">
@@ -29336,12 +29333,12 @@
         <v>106</v>
       </c>
       <c r="G41" s="109" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="151" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C42" s="335" t="n">
         <v>1</v>
@@ -29365,7 +29362,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="151" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C43" s="335" t="n">
         <v>2</v>
@@ -29389,7 +29386,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="151" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C44" s="335" t="n">
         <v>3</v>
@@ -29413,10 +29410,10 @@
     </row>
     <row r="45" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="151" t="s">
+        <v>584</v>
+      </c>
+      <c r="C45" s="341" t="s">
         <v>585</v>
-      </c>
-      <c r="C45" s="341" t="s">
-        <v>586</v>
       </c>
       <c r="D45" s="343"/>
       <c r="E45" s="31"/>
@@ -29425,7 +29422,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="151" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C46" s="333" t="str">
         <f aca="false">A43</f>
@@ -29438,7 +29435,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="151" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C47" s="333"/>
       <c r="D47" s="333"/>
@@ -29448,7 +29445,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="151" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C48" s="333"/>
       <c r="D48" s="333"/>
@@ -29458,7 +29455,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="151" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C49" s="333"/>
       <c r="D49" s="333"/>
@@ -29468,7 +29465,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="151" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C50" s="333"/>
       <c r="D50" s="333"/>
@@ -29478,7 +29475,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="151" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C51" s="333"/>
       <c r="D51" s="333"/>
@@ -29488,7 +29485,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="151" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C52" s="333"/>
       <c r="D52" s="333"/>
@@ -29498,7 +29495,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="151" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C53" s="333"/>
       <c r="D53" s="333"/>
@@ -29508,7 +29505,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="151" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C54" s="333"/>
       <c r="D54" s="333"/>
@@ -29518,7 +29515,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="151" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C55" s="333"/>
       <c r="D55" s="333"/>
@@ -29528,10 +29525,10 @@
     </row>
     <row r="56" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="151" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C56" s="334" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D56" s="334"/>
       <c r="E56" s="334"/>
@@ -29540,7 +29537,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="151" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C57" s="335" t="n">
         <v>1</v>
@@ -29555,7 +29552,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="151" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C58" s="335" t="n">
         <v>2</v>
@@ -29570,7 +29567,7 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="151" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C59" s="335" t="n">
         <v>3</v>
@@ -29585,25 +29582,25 @@
     </row>
     <row r="60" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="151" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C60" s="337"/>
       <c r="D60" s="338" t="s">
+        <v>554</v>
+      </c>
+      <c r="E60" s="338" t="s">
         <v>555</v>
       </c>
-      <c r="E60" s="338" t="s">
+      <c r="F60" s="338" t="s">
         <v>556</v>
       </c>
-      <c r="F60" s="338" t="s">
+      <c r="G60" s="339" t="s">
         <v>557</v>
-      </c>
-      <c r="G60" s="339" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="151" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C61" s="337"/>
       <c r="D61" s="109" t="s">
@@ -29616,7 +29613,7 @@
         <v>106</v>
       </c>
       <c r="G61" s="109" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29847,8 +29844,8 @@
   </sheetPr>
   <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G58" activeCellId="0" sqref="G58"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J58" activeCellId="0" sqref="J58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29869,10 +29866,10 @@
     </row>
     <row r="2" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="327" t="s">
+        <v>602</v>
+      </c>
+      <c r="C2" s="332" t="s">
         <v>603</v>
-      </c>
-      <c r="C2" s="332" t="s">
-        <v>604</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="168"/>
@@ -29881,7 +29878,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="327" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C3" s="333" t="str">
         <f aca="false">A3</f>
@@ -29894,7 +29891,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="327" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C4" s="333"/>
       <c r="D4" s="333"/>
@@ -29904,7 +29901,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="327" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C5" s="333"/>
       <c r="D5" s="333"/>
@@ -29914,7 +29911,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="327" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C6" s="333"/>
       <c r="D6" s="333"/>
@@ -29924,7 +29921,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="327" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C7" s="333"/>
       <c r="D7" s="333"/>
@@ -29934,7 +29931,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="327" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C8" s="333"/>
       <c r="D8" s="333"/>
@@ -29944,7 +29941,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="327" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="C9" s="333"/>
       <c r="D9" s="333"/>
@@ -29954,7 +29951,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="327" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C10" s="333"/>
       <c r="D10" s="333"/>
@@ -29964,7 +29961,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="327" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C11" s="333"/>
       <c r="D11" s="333"/>
@@ -29974,7 +29971,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="327" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C12" s="333"/>
       <c r="D12" s="333"/>
@@ -29984,10 +29981,10 @@
     </row>
     <row r="13" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="151" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C13" s="334" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D13" s="334"/>
       <c r="E13" s="334"/>
@@ -29996,7 +29993,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="151" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C14" s="335" t="n">
         <v>1</v>
@@ -30011,7 +30008,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="151" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C15" s="335" t="n">
         <v>2</v>
@@ -30026,7 +30023,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="151" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C16" s="335" t="n">
         <v>3</v>
@@ -30041,25 +30038,25 @@
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="151" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C17" s="337"/>
       <c r="D17" s="338" t="s">
+        <v>554</v>
+      </c>
+      <c r="E17" s="338" t="s">
         <v>555</v>
       </c>
-      <c r="E17" s="338" t="s">
+      <c r="F17" s="338" t="s">
         <v>556</v>
       </c>
-      <c r="F17" s="338" t="s">
+      <c r="G17" s="339" t="s">
         <v>557</v>
-      </c>
-      <c r="G17" s="339" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="151" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C18" s="337"/>
       <c r="D18" s="109" t="s">
@@ -30072,12 +30069,12 @@
         <v>106</v>
       </c>
       <c r="G18" s="109" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="151" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C19" s="335" t="n">
         <v>1</v>
@@ -30101,7 +30098,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="151" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C20" s="335" t="n">
         <v>2</v>
@@ -30125,7 +30122,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="151" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C21" s="335" t="n">
         <v>3</v>
@@ -30149,10 +30146,10 @@
     </row>
     <row r="22" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="151" t="s">
+        <v>623</v>
+      </c>
+      <c r="C22" s="341" t="s">
         <v>624</v>
-      </c>
-      <c r="C22" s="341" t="s">
-        <v>625</v>
       </c>
       <c r="D22" s="343"/>
       <c r="E22" s="31"/>
@@ -30161,7 +30158,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="151" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C23" s="333" t="str">
         <f aca="false">A23</f>
@@ -30174,7 +30171,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="151" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C24" s="333"/>
       <c r="D24" s="333"/>
@@ -30184,7 +30181,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="151" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C25" s="333"/>
       <c r="D25" s="333"/>
@@ -30194,7 +30191,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="151" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C26" s="333"/>
       <c r="D26" s="333"/>
@@ -30204,7 +30201,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="151" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C27" s="333"/>
       <c r="D27" s="333"/>
@@ -30214,7 +30211,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="151" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C28" s="333"/>
       <c r="D28" s="333"/>
@@ -30224,7 +30221,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="151" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C29" s="333"/>
       <c r="D29" s="333"/>
@@ -30234,7 +30231,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="151" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C30" s="333"/>
       <c r="D30" s="333"/>
@@ -30244,7 +30241,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="151" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C31" s="333"/>
       <c r="D31" s="333"/>
@@ -30254,7 +30251,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="151" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C32" s="333"/>
       <c r="D32" s="333"/>
@@ -30264,10 +30261,10 @@
     </row>
     <row r="33" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="151" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C33" s="334" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D33" s="334"/>
       <c r="E33" s="334"/>
@@ -30276,7 +30273,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="151" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C34" s="335" t="n">
         <v>1</v>
@@ -30291,7 +30288,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="151" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C35" s="335" t="n">
         <v>2</v>
@@ -30306,7 +30303,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="151" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="C36" s="335" t="n">
         <v>3</v>
@@ -30321,25 +30318,25 @@
     </row>
     <row r="37" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="151" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C37" s="337"/>
       <c r="D37" s="338" t="s">
+        <v>554</v>
+      </c>
+      <c r="E37" s="338" t="s">
         <v>555</v>
       </c>
-      <c r="E37" s="338" t="s">
+      <c r="F37" s="338" t="s">
         <v>556</v>
       </c>
-      <c r="F37" s="338" t="s">
+      <c r="G37" s="339" t="s">
         <v>557</v>
-      </c>
-      <c r="G37" s="339" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="151" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C38" s="337"/>
       <c r="D38" s="109" t="s">
@@ -30352,12 +30349,12 @@
         <v>106</v>
       </c>
       <c r="G38" s="109" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="151" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C39" s="335" t="n">
         <v>1</v>
@@ -30381,7 +30378,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="151" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C40" s="335" t="n">
         <v>2</v>
@@ -30405,7 +30402,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="151" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C41" s="335" t="n">
         <v>3</v>
@@ -30429,10 +30426,10 @@
     </row>
     <row r="42" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="151" t="s">
+        <v>644</v>
+      </c>
+      <c r="C42" s="341" t="s">
         <v>645</v>
-      </c>
-      <c r="C42" s="341" t="s">
-        <v>646</v>
       </c>
       <c r="D42" s="343"/>
       <c r="E42" s="31"/>
@@ -30441,7 +30438,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="151" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C43" s="333" t="str">
         <f aca="false">A43</f>
@@ -30454,7 +30451,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="151" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C44" s="333"/>
       <c r="D44" s="333"/>
@@ -30464,7 +30461,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="151" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="C45" s="333"/>
       <c r="D45" s="333"/>
@@ -30570,7 +30567,7 @@
     </row>
     <row r="58" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C58" s="332" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="D58" s="95"/>
       <c r="E58" s="168"/>
@@ -30588,7 +30585,7 @@
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="151"/>
       <c r="C60" s="308" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="D60" s="308"/>
       <c r="E60" s="308"/>
@@ -30780,10 +30777,10 @@
     </row>
     <row r="2" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="151" t="s">
+        <v>651</v>
+      </c>
+      <c r="C2" s="347" t="s">
         <v>652</v>
-      </c>
-      <c r="C2" s="347" t="s">
-        <v>653</v>
       </c>
       <c r="D2" s="347"/>
       <c r="E2" s="347"/>
@@ -30794,7 +30791,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="327" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C3" s="333" t="str">
         <f aca="false">A3</f>

</xml_diff>

<commit_message>
Add usage of luokittelu service for muu, mikä -values in complete energiatodistus
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-2013-sv.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-2013-sv.xlsx
@@ -8760,9 +8760,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>247320</xdr:colOff>
+      <xdr:colOff>246960</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>261000</xdr:rowOff>
+      <xdr:rowOff>260640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8776,7 +8776,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4199040"/>
-          <a:ext cx="757080" cy="213480"/>
+          <a:ext cx="756720" cy="213120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8797,9 +8797,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>147240</xdr:colOff>
+      <xdr:colOff>146880</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>261000</xdr:rowOff>
+      <xdr:rowOff>260640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8813,7 +8813,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4513320"/>
-          <a:ext cx="1100160" cy="213480"/>
+          <a:ext cx="1099800" cy="213120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8834,9 +8834,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>20520</xdr:colOff>
+      <xdr:colOff>20160</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>262080</xdr:rowOff>
+      <xdr:rowOff>261720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8850,7 +8850,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4828680"/>
-          <a:ext cx="1407240" cy="213480"/>
+          <a:ext cx="1406880" cy="213120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8871,9 +8871,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>344520</xdr:colOff>
+      <xdr:colOff>344160</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>262080</xdr:rowOff>
+      <xdr:rowOff>261720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8887,7 +8887,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5142960"/>
-          <a:ext cx="1731240" cy="213480"/>
+          <a:ext cx="1730880" cy="213120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8908,9 +8908,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>217800</xdr:colOff>
+      <xdr:colOff>217440</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>275040</xdr:rowOff>
+      <xdr:rowOff>274680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8924,7 +8924,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5457240"/>
-          <a:ext cx="2038320" cy="226440"/>
+          <a:ext cx="2037960" cy="226080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8945,9 +8945,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>160920</xdr:colOff>
+      <xdr:colOff>160560</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>262080</xdr:rowOff>
+      <xdr:rowOff>261720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8961,7 +8961,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5771520"/>
-          <a:ext cx="2383200" cy="213480"/>
+          <a:ext cx="2382840" cy="213120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8982,9 +8982,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>101160</xdr:colOff>
+      <xdr:colOff>100800</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>261000</xdr:rowOff>
+      <xdr:rowOff>260640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8998,7 +8998,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="6085080"/>
-          <a:ext cx="2696400" cy="213480"/>
+          <a:ext cx="2696040" cy="213120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9398,9 +9398,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>317520</xdr:colOff>
+      <xdr:colOff>317160</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>78480</xdr:rowOff>
+      <xdr:rowOff>78120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9410,7 +9410,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1994400" y="149040"/>
-          <a:ext cx="6999480" cy="10062720"/>
+          <a:ext cx="6999120" cy="10062360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9496,9 +9496,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>5400</xdr:colOff>
+      <xdr:colOff>5040</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>79560</xdr:rowOff>
+      <xdr:rowOff>79200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9508,7 +9508,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1987560" y="10344960"/>
-          <a:ext cx="7016760" cy="266400"/>
+          <a:ext cx="7016400" cy="266040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9562,9 +9562,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>433800</xdr:colOff>
+      <xdr:colOff>433440</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>56880</xdr:rowOff>
+      <xdr:rowOff>56520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9574,7 +9574,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5525280" y="4883760"/>
-          <a:ext cx="795600" cy="267480"/>
+          <a:ext cx="795240" cy="267120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9626,9 +9626,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>432720</xdr:colOff>
+      <xdr:colOff>432360</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>196560</xdr:rowOff>
+      <xdr:rowOff>196200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9638,7 +9638,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5524200" y="5023440"/>
-          <a:ext cx="795600" cy="267480"/>
+          <a:ext cx="795240" cy="267120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -22340,7 +22340,7 @@
   <dimension ref="A1:N94"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+      <selection pane="topLeft" activeCell="M59" activeCellId="0" sqref="M59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23296,8 +23296,8 @@
         <v>260</v>
       </c>
       <c r="E53" s="199" t="str">
-        <f aca="false">A64</f>
-        <v>[:lahtotiedot :lammitys :label-fi]</v>
+        <f aca="false">A65</f>
+        <v>[:lahtotiedot :lammitys :label-sv]</v>
       </c>
       <c r="F53" s="199"/>
       <c r="G53" s="199"/>

</xml_diff>

<commit_message>
AE-579 fix wrong field in xlsx template
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-2013-sv.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-2013-sv.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="1) etusivu" sheetId="1" state="visible" r:id="rId2"/>
@@ -2188,6 +2188,7 @@
         <color rgb="FF009EE0"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">m</t>
     </r>
@@ -2199,6 +2200,7 @@
         <color rgb="FF009EE0"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
@@ -3360,7 +3362,7 @@
     <numFmt numFmtId="173" formatCode="#,##0.00"/>
     <numFmt numFmtId="174" formatCode="0.0"/>
   </numFmts>
-  <fonts count="41">
+  <fonts count="39">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -3630,21 +3632,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF009EE0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <vertAlign val="superscript"/>
-      <sz val="10"/>
-      <color rgb="FF009EE0"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -5101,11 +5088,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5133,7 +5120,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="39" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="37" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5225,7 +5212,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="39" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="37" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5301,11 +5288,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="40" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="40" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -8798,9 +8785,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>246240</xdr:colOff>
+      <xdr:colOff>245880</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>259920</xdr:rowOff>
+      <xdr:rowOff>259560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8814,7 +8801,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4199040"/>
-          <a:ext cx="756000" cy="212400"/>
+          <a:ext cx="755640" cy="212040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8835,9 +8822,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>146160</xdr:colOff>
+      <xdr:colOff>145800</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>259920</xdr:rowOff>
+      <xdr:rowOff>259560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8851,7 +8838,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4513320"/>
-          <a:ext cx="1099080" cy="212400"/>
+          <a:ext cx="1098720" cy="212040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8872,9 +8859,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>19440</xdr:colOff>
+      <xdr:colOff>19080</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>261000</xdr:rowOff>
+      <xdr:rowOff>260640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8888,7 +8875,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4828680"/>
-          <a:ext cx="1406160" cy="212400"/>
+          <a:ext cx="1405800" cy="212040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8909,9 +8896,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>343440</xdr:colOff>
+      <xdr:colOff>343080</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>261000</xdr:rowOff>
+      <xdr:rowOff>260640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8925,7 +8912,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5142960"/>
-          <a:ext cx="1730160" cy="212400"/>
+          <a:ext cx="1729800" cy="212040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8946,9 +8933,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>216720</xdr:colOff>
+      <xdr:colOff>216360</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>273960</xdr:rowOff>
+      <xdr:rowOff>273600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8962,7 +8949,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5457240"/>
-          <a:ext cx="2037240" cy="225360"/>
+          <a:ext cx="2036880" cy="225000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8983,9 +8970,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>159840</xdr:colOff>
+      <xdr:colOff>159480</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>261000</xdr:rowOff>
+      <xdr:rowOff>260640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8999,7 +8986,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5771520"/>
-          <a:ext cx="2382120" cy="212400"/>
+          <a:ext cx="2381760" cy="212040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9020,9 +9007,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>100080</xdr:colOff>
+      <xdr:colOff>99720</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>259920</xdr:rowOff>
+      <xdr:rowOff>259560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9036,7 +9023,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="6085080"/>
-          <a:ext cx="2695320" cy="212400"/>
+          <a:ext cx="2694960" cy="212040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9436,9 +9423,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>316440</xdr:colOff>
+      <xdr:colOff>316080</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>77400</xdr:rowOff>
+      <xdr:rowOff>77040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9448,7 +9435,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1994400" y="149040"/>
-          <a:ext cx="6998400" cy="10061640"/>
+          <a:ext cx="6998040" cy="10061280"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9534,9 +9521,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>4320</xdr:colOff>
+      <xdr:colOff>3960</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>78480</xdr:rowOff>
+      <xdr:rowOff>78120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9546,7 +9533,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1987560" y="10344960"/>
-          <a:ext cx="7015680" cy="265320"/>
+          <a:ext cx="7015320" cy="264960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9600,9 +9587,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>432720</xdr:colOff>
+      <xdr:colOff>432360</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>55800</xdr:rowOff>
+      <xdr:rowOff>55440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9612,7 +9599,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5525280" y="4883760"/>
-          <a:ext cx="794520" cy="266400"/>
+          <a:ext cx="794160" cy="266040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9664,9 +9651,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>431640</xdr:colOff>
+      <xdr:colOff>431280</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>195480</xdr:rowOff>
+      <xdr:rowOff>195120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9676,7 +9663,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5524200" y="5023440"/>
-          <a:ext cx="794520" cy="266400"/>
+          <a:ext cx="794160" cy="266040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -27337,7 +27324,7 @@
   </sheetPr>
   <dimension ref="A1:Y67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -27346,8 +27333,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="90" width="61.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="26" width="0.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="26" width="1.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="26" width="23.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="26" width="7.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="26" width="23.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="26" width="7.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="26" width="15.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="7" style="26" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="26" width="2.42"/>
@@ -27441,10 +27428,10 @@
         <v>448</v>
       </c>
       <c r="C7" s="97"/>
-      <c r="D7" s="274" t="s">
+      <c r="D7" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="E7" s="29" t="str">
+      <c r="E7" s="274" t="str">
         <f aca="false">A3</f>
         <v>#function[solita.etp.service.energiatodistus-pdf/fn--61283]</v>
       </c>
@@ -29246,7 +29233,7 @@
   </sheetPr>
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J61" activeCellId="0" sqref="J61"/>
     </sheetView>
   </sheetViews>
@@ -30298,8 +30285,8 @@
   </sheetPr>
   <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J59" activeCellId="0" sqref="J59"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -30763,8 +30750,8 @@
         <v>3</v>
       </c>
       <c r="D36" s="344" t="str">
-        <f aca="false">A28</f>
-        <v>[:huomiot :valaistus-muut :toimenpide 2 :nimi-fi]</v>
+        <f aca="false">A29</f>
+        <v>[:huomiot :valaistus-muut :toimenpide 2 :nimi-sv]</v>
       </c>
       <c r="E36" s="344"/>
       <c r="F36" s="344"/>

</xml_diff>

<commit_message>
AE-980 fix e-luokka table in xlsx template
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-2013-sv.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-2013-sv.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1) etusivu" sheetId="1" state="visible" r:id="rId2"/>
@@ -4563,15 +4563,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="25" fillId="7" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="25" fillId="7" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="25" fillId="8" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="25" fillId="8" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="15" fillId="9" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="9" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -8810,9 +8810,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>243360</xdr:colOff>
+      <xdr:colOff>243000</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>257040</xdr:rowOff>
+      <xdr:rowOff>256680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8826,7 +8826,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4199040"/>
-          <a:ext cx="753120" cy="209520"/>
+          <a:ext cx="752760" cy="209160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8847,9 +8847,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>143280</xdr:colOff>
+      <xdr:colOff>142920</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>257040</xdr:rowOff>
+      <xdr:rowOff>256680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8863,7 +8863,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4513320"/>
-          <a:ext cx="1096200" cy="209520"/>
+          <a:ext cx="1095840" cy="209160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8884,9 +8884,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>16560</xdr:colOff>
+      <xdr:colOff>16200</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>258120</xdr:rowOff>
+      <xdr:rowOff>257760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8900,7 +8900,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4828680"/>
-          <a:ext cx="1403280" cy="209520"/>
+          <a:ext cx="1402920" cy="209160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8921,9 +8921,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>340560</xdr:colOff>
+      <xdr:colOff>340200</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>258120</xdr:rowOff>
+      <xdr:rowOff>257760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8937,7 +8937,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5142960"/>
-          <a:ext cx="1727280" cy="209520"/>
+          <a:ext cx="1726920" cy="209160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8958,9 +8958,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>213840</xdr:colOff>
+      <xdr:colOff>213480</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>271080</xdr:rowOff>
+      <xdr:rowOff>270720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8974,7 +8974,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5457240"/>
-          <a:ext cx="2034360" cy="222480"/>
+          <a:ext cx="2034000" cy="222120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8995,9 +8995,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>156960</xdr:colOff>
+      <xdr:colOff>156600</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>258120</xdr:rowOff>
+      <xdr:rowOff>257760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9011,7 +9011,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5771520"/>
-          <a:ext cx="2379240" cy="209520"/>
+          <a:ext cx="2378880" cy="209160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9032,9 +9032,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>97200</xdr:colOff>
+      <xdr:colOff>96840</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>257040</xdr:rowOff>
+      <xdr:rowOff>256680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9048,7 +9048,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="6085080"/>
-          <a:ext cx="2692440" cy="209520"/>
+          <a:ext cx="2692080" cy="209160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9448,9 +9448,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>313560</xdr:colOff>
+      <xdr:colOff>313200</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>74520</xdr:rowOff>
+      <xdr:rowOff>74160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9460,7 +9460,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1994400" y="149040"/>
-          <a:ext cx="6995520" cy="10058760"/>
+          <a:ext cx="6995160" cy="10058400"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9546,9 +9546,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>1440</xdr:colOff>
+      <xdr:colOff>1080</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>75600</xdr:rowOff>
+      <xdr:rowOff>75240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9558,7 +9558,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1987560" y="10344960"/>
-          <a:ext cx="7012800" cy="262440"/>
+          <a:ext cx="7012440" cy="262080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9612,9 +9612,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>429840</xdr:colOff>
+      <xdr:colOff>429480</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>52920</xdr:rowOff>
+      <xdr:rowOff>52560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9624,7 +9624,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5525280" y="4883760"/>
-          <a:ext cx="791640" cy="263520"/>
+          <a:ext cx="791280" cy="263160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9676,9 +9676,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>428760</xdr:colOff>
+      <xdr:colOff>428400</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>192600</xdr:rowOff>
+      <xdr:rowOff>192240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9688,7 +9688,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5524200" y="5023440"/>
-          <a:ext cx="791640" cy="263520"/>
+          <a:ext cx="791280" cy="263160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9741,8 +9741,8 @@
   </sheetPr>
   <dimension ref="A1:AK262"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S28" activeCellId="0" sqref="S28"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19556,8 +19556,8 @@
   </sheetPr>
   <dimension ref="A1:AC82"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D35" activeCellId="0" sqref="D35"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M43" activeCellId="0" sqref="M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20614,16 +20614,16 @@
       <c r="E30" s="61"/>
       <c r="F30" s="14"/>
       <c r="H30" s="135" t="str">
-        <f aca="false">A40</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--64381]</v>
-      </c>
-      <c r="I30" s="136" t="str">
-        <f aca="false">A41</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--64384]</v>
-      </c>
-      <c r="J30" s="137" t="str">
         <f aca="false">A42</f>
         <v>#function[solita.etp.service.energiatodistus-pdf/fn--64387]</v>
+      </c>
+      <c r="I30" s="136" t="str">
+        <f aca="false">A43</f>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--64390]</v>
+      </c>
+      <c r="J30" s="137" t="str">
+        <f aca="false">A44</f>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--64393]</v>
       </c>
       <c r="K30" s="130"/>
       <c r="M30" s="0"/>

</xml_diff>

<commit_message>
AE-1481 Improve Swedish translation of ET sheet
energiformsfaktor -> energiformsfaktorn
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-2013-sv.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-2013-sv.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1) etusivu" sheetId="1" state="visible" r:id="rId2"/>
@@ -407,7 +407,7 @@
     <t xml:space="preserve">Energiforms-faktor</t>
   </si>
   <si>
-    <t xml:space="preserve">Energimängd viktad med energiformsfaktor</t>
+    <t xml:space="preserve">Energimängd viktad med energiformsfaktorn</t>
   </si>
   <si>
     <t xml:space="preserve">[:tulokset :kaytettavat-energiamuodot :kaukolampo-nettoala]</t>
@@ -8757,9 +8757,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>241920</xdr:colOff>
+      <xdr:colOff>241560</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>255600</xdr:rowOff>
+      <xdr:rowOff>255240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8773,12 +8773,12 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4199040"/>
-          <a:ext cx="751680" cy="208080"/>
+          <a:ext cx="751320" cy="207720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -8794,9 +8794,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>141840</xdr:colOff>
+      <xdr:colOff>141480</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>255600</xdr:rowOff>
+      <xdr:rowOff>255240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8810,12 +8810,12 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4513320"/>
-          <a:ext cx="1094760" cy="208080"/>
+          <a:ext cx="1094400" cy="207720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -8831,9 +8831,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>15120</xdr:colOff>
+      <xdr:colOff>14760</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>256680</xdr:rowOff>
+      <xdr:rowOff>256320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8847,12 +8847,12 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4828680"/>
-          <a:ext cx="1401840" cy="208080"/>
+          <a:ext cx="1401480" cy="207720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -8868,9 +8868,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>339120</xdr:colOff>
+      <xdr:colOff>338760</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>256680</xdr:rowOff>
+      <xdr:rowOff>256320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8884,12 +8884,12 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5142960"/>
-          <a:ext cx="1725840" cy="208080"/>
+          <a:ext cx="1725480" cy="207720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -8905,9 +8905,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>212400</xdr:colOff>
+      <xdr:colOff>212040</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>269640</xdr:rowOff>
+      <xdr:rowOff>269280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8921,12 +8921,12 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5457240"/>
-          <a:ext cx="2032920" cy="221040"/>
+          <a:ext cx="2032560" cy="220680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -8942,9 +8942,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>155520</xdr:colOff>
+      <xdr:colOff>155160</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>256680</xdr:rowOff>
+      <xdr:rowOff>256320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8958,12 +8958,12 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5771520"/>
-          <a:ext cx="2377800" cy="208080"/>
+          <a:ext cx="2377440" cy="207720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -8979,9 +8979,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>95760</xdr:colOff>
+      <xdr:colOff>95400</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>255600</xdr:rowOff>
+      <xdr:rowOff>255240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8995,12 +8995,12 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="6085080"/>
-          <a:ext cx="2691000" cy="208080"/>
+          <a:ext cx="2690640" cy="207720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -9349,13 +9349,13 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>294120</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>60120</xdr:rowOff>
+      <xdr:rowOff>60480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>294120</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>52560</xdr:rowOff>
+      <xdr:rowOff>52920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9395,9 +9395,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>312120</xdr:colOff>
+      <xdr:colOff>311760</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>73080</xdr:rowOff>
+      <xdr:rowOff>72720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9407,7 +9407,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1994400" y="149040"/>
-          <a:ext cx="6994080" cy="10057320"/>
+          <a:ext cx="6993720" cy="10056960"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9493,9 +9493,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>322560</xdr:colOff>
+      <xdr:colOff>322200</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>74160</xdr:rowOff>
+      <xdr:rowOff>73800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9505,7 +9505,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1987560" y="10344960"/>
-          <a:ext cx="7011360" cy="261000"/>
+          <a:ext cx="7011000" cy="260640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9524,7 +9524,7 @@
         <a:fontRef idx="minor"/>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr lIns="90000" rIns="90000" tIns="45000" bIns="45000">
+        <a:bodyPr lIns="90000" rIns="90000" tIns="45000" bIns="45000" anchor="t">
           <a:noAutofit/>
         </a:bodyPr>
         <a:p>
@@ -9542,7 +9542,7 @@
             </a:rPr>
             <a:t>Energicertifikatet grundar sig på lagen om energicertifikat för byggnader  (50/2013). </a:t>
           </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+          <a:endParaRPr b="0" lang="fi-FI" sz="1100" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
@@ -9559,9 +9559,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>428400</xdr:colOff>
+      <xdr:colOff>428040</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>51480</xdr:rowOff>
+      <xdr:rowOff>51120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9571,13 +9571,13 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5525280" y="4883760"/>
-          <a:ext cx="790200" cy="262080"/>
+          <a:ext cx="789840" cy="261720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -9606,7 +9606,7 @@
             </a:rPr>
             <a:t>Normnivån för</a:t>
           </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="700" spc="-1" strike="noStrike">
+          <a:endParaRPr b="0" lang="fi-FI" sz="700" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
@@ -9623,9 +9623,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>427320</xdr:colOff>
+      <xdr:colOff>426960</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>191160</xdr:rowOff>
+      <xdr:rowOff>190800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9635,13 +9635,13 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5524200" y="5023440"/>
-          <a:ext cx="790200" cy="262080"/>
+          <a:ext cx="789840" cy="261720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -9670,7 +9670,7 @@
             </a:rPr>
             <a:t>nybyggnader 2012</a:t>
           </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="700" spc="-1" strike="noStrike">
+          <a:endParaRPr b="0" lang="fi-FI" sz="700" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
@@ -19476,18 +19476,18 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B9:H11 J9:AMJ9 I10:AMJ11" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B9:H11 J9:AMJ9 I10:AMJ11" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A9:A11" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A9:A11" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
-  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -19503,8 +19503,8 @@
   </sheetPr>
   <dimension ref="A1:AC82"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M43" activeCellId="0" sqref="M43"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22270,8 +22270,8 @@
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
-  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -22286,7 +22286,7 @@
   </sheetPr>
   <dimension ref="A1:N94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D75" activeCellId="0" sqref="D75"/>
     </sheetView>
   </sheetViews>
@@ -24646,14 +24646,14 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A49:E49 G49:AMJ49" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A49:E49 G49:AMJ49" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
-  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -27205,14 +27205,14 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H44:H47 G47 G49:H49" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H44:H47 G47 G49:H49" type="none">
       <formula1>OR(ISNUMBER(#ref!),#ref!="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
-  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -29120,8 +29120,8 @@
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
-  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -30164,14 +30164,14 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A63:F64 H63:AMJ64 G64" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A63:F64 H63:AMJ64 G64" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
-  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -31081,8 +31081,8 @@
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
-  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -32283,8 +32283,8 @@
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
-  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>